<commit_message>
Se crean nuevos metodos para automatizar epos
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>MSIDN</t>
   </si>
@@ -119,16 +119,25 @@
     <t>732111198172293</t>
   </si>
   <si>
-    <t>3016877412</t>
-  </si>
-  <si>
-    <t>3016876877</t>
-  </si>
-  <si>
     <t>MSI</t>
   </si>
   <si>
     <t>732111198172294</t>
+  </si>
+  <si>
+    <t>8957732111198172293</t>
+  </si>
+  <si>
+    <t>8957732111198172292</t>
+  </si>
+  <si>
+    <t>3016876876</t>
+  </si>
+  <si>
+    <t>3016877591</t>
+  </si>
+  <si>
+    <t>732111198172292</t>
   </si>
 </sst>
 </file>
@@ -527,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -683,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="6"/>
@@ -703,7 +712,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="6"/>
@@ -717,10 +726,10 @@
         <v>3003324</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3016876876</v>
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>30</v>
@@ -731,29 +740,16 @@
         <v>3003324</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="1">
-        <v>3003324</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>

</xml_diff>

<commit_message>
se actualiza repositorio con las clases para manejo de winwap y cargue de inventario, se cambia el nombre de las clases para seguir con el esquema de diseño.
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PrepaidAutomation\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E100FAE-4FD5-428E-BC48-70AAD6E5DFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3470" yWindow="3470" windowWidth="21600" windowHeight="11390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -143,8 +144,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,13 +175,6 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -203,7 +197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -220,7 +214,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -535,24 +532,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="38.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.54296875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -658,28 +655,25 @@
       <c r="D7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="7"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
@@ -694,12 +688,11 @@
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1">
@@ -714,12 +707,11 @@
       <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1">
@@ -749,12 +741,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>